<commit_message>
updates to boost::nowide 11.3.0
</commit_message>
<xml_diff>
--- a/SlicerLibraries.xlsx
+++ b/SlicerLibraries.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
   <si>
     <t xml:space="preserve">Version old</t>
   </si>
@@ -236,6 +236,111 @@
   </si>
   <si>
     <t xml:space="preserve">1.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> admesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> agg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> angelscript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.35.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.37.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ankerl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.4.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> avrdude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015(?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> boost nowide</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> build-utils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTF-8 code check</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> clipper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> exif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exif data from JPEG</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fast_float</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> glu-libtess</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hidapi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hints</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> imgui</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jpeg-compressor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> libigl</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> libnest2d</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> miniz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nlohmann</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> occt_wrapper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> qhull</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> qoi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> semver</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> stb_dxt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tcbspan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> test-utils</t>
   </si>
 </sst>
 </file>
@@ -319,7 +424,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -332,12 +437,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -357,18 +466,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="35.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,6 +860,285 @@
       <c r="D26" s="2"/>
       <c r="E26" s="3"/>
     </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="3" t="n">
+        <v>2005</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="3" t="n">
+        <v>2002</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="3"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
updates to Eigen 3.4.0 3147391d
</commit_message>
<xml_diff>
--- a/SlicerLibraries.xlsx
+++ b/SlicerLibraries.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="110">
   <si>
     <t xml:space="preserve">Version old</t>
   </si>
@@ -271,6 +271,9 @@
     <t xml:space="preserve"> boost nowide</t>
   </si>
   <si>
+    <t xml:space="preserve">11.3.0</t>
+  </si>
+  <si>
     <t xml:space="preserve"> build-utils</t>
   </si>
   <si>
@@ -281,6 +284,12 @@
   </si>
   <si>
     <t xml:space="preserve"> eigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3.7 323c052e1731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.4.0</t>
   </si>
   <si>
     <t xml:space="preserve"> exif</t>
@@ -424,7 +433,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -443,10 +452,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -468,8 +473,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -866,7 +871,7 @@
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="2"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,7 +884,7 @@
       <c r="C31" s="3" t="n">
         <v>2.4</v>
       </c>
-      <c r="D31" s="5"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -892,7 +897,7 @@
       <c r="C32" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="3"/>
@@ -907,7 +912,7 @@
       <c r="C33" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E33" s="3"/>
@@ -920,7 +925,7 @@
         <v>81</v>
       </c>
       <c r="C34" s="3"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="2"/>
       <c r="E34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,214 +933,224 @@
         <v>82</v>
       </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B36" s="3" t="n">
         <v>2005</v>
       </c>
       <c r="C36" s="3"/>
-      <c r="D36" s="5"/>
+      <c r="D36" s="2"/>
       <c r="E36" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
-      <c r="D37" s="5"/>
+      <c r="D37" s="2"/>
       <c r="E37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="2"/>
       <c r="E38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B39" s="3" t="n">
         <v>2002</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="5"/>
+      <c r="C39" s="3" t="n">
+        <v>2002</v>
+      </c>
+      <c r="D39" s="2"/>
       <c r="E39" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="D40" s="5"/>
+      <c r="D40" s="2"/>
       <c r="E40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="D41" s="5"/>
+      <c r="D41" s="2"/>
       <c r="E41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="2"/>
       <c r="E42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="2"/>
       <c r="E43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
-      <c r="D44" s="5"/>
+      <c r="D44" s="2"/>
       <c r="E44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="5"/>
+      <c r="D45" s="2"/>
       <c r="E45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="5"/>
+      <c r="D46" s="2"/>
       <c r="E46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="5"/>
+      <c r="D47" s="2"/>
       <c r="E47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="5"/>
+      <c r="D48" s="2"/>
       <c r="E48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
-      <c r="D49" s="5"/>
+      <c r="D49" s="2"/>
       <c r="E49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="5"/>
+      <c r="D50" s="2"/>
       <c r="E50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
-      <c r="D51" s="5"/>
+      <c r="D51" s="2"/>
       <c r="E51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="5"/>
+      <c r="D52" s="2"/>
       <c r="E52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
-      <c r="D53" s="5"/>
+      <c r="D53" s="2"/>
       <c r="E53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
-      <c r="D54" s="5"/>
+      <c r="D54" s="2"/>
       <c r="E54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
-      <c r="D55" s="5"/>
+      <c r="D55" s="2"/>
       <c r="E55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
-      <c r="D56" s="5"/>
+      <c r="D56" s="2"/>
       <c r="E56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
-      <c r="D57" s="5"/>
+      <c r="D57" s="2"/>
       <c r="E57" s="3"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>